<commit_message>
Updated TCs and added new functions with test data file.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/renameFolder_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/renameFolder_newUI/TestData.xlsx
@@ -12,44 +12,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
+    <t>URL_login_login</t>
+  </si>
+  <si>
     <t>GoogleChrome</t>
   </si>
   <si>
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
+    <t>#/login</t>
+  </si>
+  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
-    <t>#/login</t>
-  </si>
-  <si>
     <t>URL_content</t>
   </si>
   <si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>汉字汉字漢字</t>
+  </si>
+  <si>
+    <t>Automation_Folder_Rename_NoRename</t>
   </si>
 </sst>
 </file>
@@ -301,11 +304,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -385,38 +388,38 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -986,9 +989,15 @@
       <c r="Z26" s="17"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -2655,79 +2664,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>